<commit_message>
update anh tuanBG + lapdat
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang2/02.XuLyBH/XLBH2302_AnhTuanBG.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang2/02.XuLyBH/XLBH2302_AnhTuanBG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4035" windowWidth="10320" windowHeight="4065" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="4035" windowWidth="10320" windowHeight="4065" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TG102V" sheetId="49" r:id="rId1"/>
@@ -6764,7 +6764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -12662,8 +12662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="M3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="M3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12878,7 +12878,9 @@
       <c r="B6" s="67">
         <v>44985</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="67">
+        <v>44999</v>
+      </c>
       <c r="D6" s="64" t="s">
         <v>63</v>
       </c>
@@ -12918,7 +12920,7 @@
       <c r="R6" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="3"/>
+      <c r="S6" s="72"/>
       <c r="T6" s="66"/>
       <c r="U6" s="88" t="s">
         <v>18</v>
@@ -12935,7 +12937,9 @@
       <c r="B7" s="67">
         <v>44985</v>
       </c>
-      <c r="C7" s="67"/>
+      <c r="C7" s="67">
+        <v>44999</v>
+      </c>
       <c r="D7" s="64" t="s">
         <v>63</v>
       </c>
@@ -12975,7 +12979,7 @@
       <c r="R7" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="S7" s="3"/>
+      <c r="S7" s="72"/>
       <c r="T7" s="66"/>
       <c r="U7" s="89"/>
       <c r="V7" s="3" t="s">
@@ -12990,7 +12994,9 @@
       <c r="B8" s="67">
         <v>44985</v>
       </c>
-      <c r="C8" s="67"/>
+      <c r="C8" s="67">
+        <v>44999</v>
+      </c>
       <c r="D8" s="64" t="s">
         <v>63</v>
       </c>
@@ -13024,13 +13030,13 @@
       <c r="P8" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="37" t="s">
+      <c r="R8" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="S8" s="3"/>
+      <c r="S8" s="72"/>
       <c r="T8" s="66"/>
       <c r="U8" s="89"/>
       <c r="V8" s="3" t="s">
@@ -13045,7 +13051,9 @@
       <c r="B9" s="67">
         <v>44985</v>
       </c>
-      <c r="C9" s="67"/>
+      <c r="C9" s="67">
+        <v>44999</v>
+      </c>
       <c r="D9" s="64" t="s">
         <v>63</v>
       </c>
@@ -13079,13 +13087,13 @@
       <c r="P9" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q9" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="R9" s="37" t="s">
+      <c r="R9" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="S9" s="3"/>
+      <c r="S9" s="72"/>
       <c r="T9" s="66"/>
       <c r="U9" s="89"/>
       <c r="V9" s="3" t="s">
@@ -13100,7 +13108,9 @@
       <c r="B10" s="67">
         <v>44985</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="67">
+        <v>44999</v>
+      </c>
       <c r="D10" s="64" t="s">
         <v>63</v>
       </c>
@@ -13134,13 +13144,13 @@
       <c r="P10" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="R10" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="S10" s="3"/>
+      <c r="S10" s="72"/>
       <c r="T10" s="66"/>
       <c r="U10" s="89"/>
       <c r="V10" s="3" t="s">
@@ -13155,7 +13165,9 @@
       <c r="B11" s="67">
         <v>44985</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="67">
+        <v>44999</v>
+      </c>
       <c r="D11" s="64" t="s">
         <v>63</v>
       </c>
@@ -13191,13 +13203,13 @@
       <c r="P11" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="R11" s="37" t="s">
+      <c r="R11" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="S11" s="3"/>
+      <c r="S11" s="72"/>
       <c r="T11" s="66"/>
       <c r="U11" s="89"/>
       <c r="V11" s="3" t="s">
@@ -13224,9 +13236,9 @@
       <c r="N12" s="70"/>
       <c r="O12" s="69"/>
       <c r="P12" s="70"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="3"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="64"/>
+      <c r="S12" s="72"/>
       <c r="T12" s="66"/>
       <c r="U12" s="88" t="s">
         <v>19</v>
@@ -13255,9 +13267,9 @@
       <c r="N13" s="70"/>
       <c r="O13" s="69"/>
       <c r="P13" s="70"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="3"/>
+      <c r="Q13" s="71"/>
+      <c r="R13" s="64"/>
+      <c r="S13" s="72"/>
       <c r="T13" s="66"/>
       <c r="U13" s="89"/>
       <c r="V13" s="3" t="s">

</xml_diff>